<commit_message>
Final commit of example code
</commit_message>
<xml_diff>
--- a/spec_by_example/cd_warehouse_by_cd.xlsx
+++ b/spec_by_example/cd_warehouse_by_cd.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="In stock, payment accepted" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -23,10 +23,100 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+  <si>
+    <t>GIVEN</t>
+  </si>
+  <si>
+    <t>WHEN</t>
+  </si>
+  <si>
+    <t>THEN</t>
+  </si>
+  <si>
+    <t>One copy is deducted from CD's stock</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>The charts are notified of the sale</t>
+  </si>
+  <si>
+    <t>The customer buy that CD</t>
+  </si>
+  <si>
+    <t>a CD that's in the Top 100 and we have it in stock, and the customer's card payment will be accepted</t>
+  </si>
+  <si>
+    <t>The customer's card is charged £1 less than the lowest price from competitors found for that CD</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>Chart Position</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Credit Card</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Payment Accepted</t>
+  </si>
+  <si>
+    <t>Lowest Price</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>title: "NumberOf The Beast", artist: "Iron Maiden"</t>
+  </si>
+  <si>
+    <t>Outputs</t>
+  </si>
+  <si>
+    <t>End Stock</t>
+  </si>
+  <si>
+    <t>Charged</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>sales: 1, album: "Iron Maiden - Number Of The Beast"</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -54,8 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -71,6 +163,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:J9" totalsRowShown="0">
+  <autoFilter ref="A8:J9"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="CD"/>
+    <tableColumn id="2" name="Chart Position"/>
+    <tableColumn id="3" name="Stock"/>
+    <tableColumn id="4" name="Price"/>
+    <tableColumn id="5" name="Credit Card"/>
+    <tableColumn id="6" name="Payment Accepted"/>
+    <tableColumn id="7" name="Lowest Price"/>
+    <tableColumn id="8" name="End Stock"/>
+    <tableColumn id="9" name="Charged"/>
+    <tableColumn id="10" name="Notification"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,12 +447,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:J9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="44.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.21875" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>9.99</v>
+      </c>
+      <c r="E9">
+        <v>1234234634564560</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>7.99</v>
+      </c>
+      <c r="H9">
+        <v>9</v>
+      </c>
+      <c r="I9">
+        <v>6.99</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>